<commit_message>
added KPIs and attribute
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX/Data/inbevtradmx_template_2.xlsx
+++ b/Projects/INBEVTRADMX/Data/inbevtradmx_template_2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,9 +15,10 @@
     <sheet name="store types" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">template!$A$1:$U$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">template!$A$1:$U$50</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">template!$A$1:$U$49</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">template!$A$1:$U$50</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">template!$A$1:$U$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">template!$A$1:$U$50</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">template!$A$1:$U$49</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -38,22 +39,25 @@
       <text>
         <r>
           <rPr>
+            <b val="true"/>
             <sz val="10"/>
-            <rFont val="Arial"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Jose Lach:
+          <t xml:space="preserve">Jose Lach:
 </t>
         </r>
         <r>
           <rPr>
             <sz val="10"/>
-            <rFont val="Arial"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>This is not regular Category, it is Categoria Tradicional (product attribute)</t>
+          <t xml:space="preserve">This is not regular Category, it is Categoria Tradicional (product attribute)</t>
         </r>
       </text>
     </comment>
@@ -62,486 +66,501 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="189">
-  <si>
-    <t>KPI Level 1 Name</t>
-  </si>
-  <si>
-    <t>KPI Level 2 Name</t>
-  </si>
-  <si>
-    <t>KPI Level 3 Name</t>
-  </si>
-  <si>
-    <t>product_type</t>
-  </si>
-  <si>
-    <t>exclude skus</t>
-  </si>
-  <si>
-    <t>product_name</t>
-  </si>
-  <si>
-    <t>Survey Question Code</t>
-  </si>
-  <si>
-    <t>Survey question</t>
-  </si>
-  <si>
-    <t>Possible Answer</t>
-  </si>
-  <si>
-    <t>manufacturer_name</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Categoria Tradicional</t>
-  </si>
-  <si>
-    <t>brand_name</t>
-  </si>
-  <si>
-    <t>weights</t>
-  </si>
-  <si>
-    <t>store_type</t>
-  </si>
-  <si>
-    <t>Store Additional Attribute 4</t>
-  </si>
-  <si>
-    <t>Store Additional Attribute 13</t>
-  </si>
-  <si>
-    <t>template_name</t>
-  </si>
-  <si>
-    <t>Pass/Fail Criteria</t>
-  </si>
-  <si>
-    <t>column names</t>
-  </si>
-  <si>
-    <t>KPI type</t>
-  </si>
-  <si>
-    <t>Set Botella Cerrada</t>
-  </si>
-  <si>
-    <t>Promociones Vigentes</t>
-  </si>
-  <si>
-    <t>POS</t>
-  </si>
-  <si>
-    <t>"Nothing to Tag", "Uniforme", "Corcholata Entrada", "Logo Modelorama Exterior", "Termometro", 2X58 1X33 MEGA CORONA LIGHT, Mega light, Premium Stella Michelob Cucapa_Sabor para conocedores, TendCardTriptico_Michelob, TendCardTriptico_Stella Artois, TendCardTriptico_Cucapa, 1X30MEGAC, 1X28MEGAC, Michelob POS Other, Stella Artois POS Other, Cucapa POS Other,</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>ABI-GM</t>
-  </si>
-  <si>
-    <t>TRADICIONAL</t>
-  </si>
-  <si>
-    <t>BC</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>POP Exterior, POP Interior</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in at least one of the scene types there is product type POS from Manufacturer ABI, then pass.</t>
-  </si>
-  <si>
-    <t>product_type, exclude skus, manufacturer_name, store_type, Store Additional Attribute 4, scene_type</t>
-  </si>
-  <si>
-    <t>Product Availability</t>
-  </si>
-  <si>
-    <t>Pureza Cooler</t>
-  </si>
-  <si>
-    <t>SKU,Other,Empty</t>
-  </si>
-  <si>
-    <t>ABI-GM, NESTLE, GARCI CRESPO, KERMATO</t>
-  </si>
-  <si>
-    <t>Cooler</t>
-  </si>
-  <si>
-    <t>Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the cooler for selected manufacturers. 100% purity target.</t>
-  </si>
-  <si>
-    <t>product_type, manufacturer_name, store_type, Store Additional Attribute 4, scene_type</t>
-  </si>
-  <si>
-    <t>SOS</t>
-  </si>
-  <si>
-    <t>Primer Impacto</t>
-  </si>
-  <si>
-    <t>Enfriador en área alto impacto 100% de productos son de GM</t>
-  </si>
-  <si>
-    <t>Si, No, No tiene Enfriador</t>
-  </si>
-  <si>
-    <t>Expected Answers: "Si" &amp; "No tiene Enfirador"</t>
-  </si>
-  <si>
-    <t>Survey Question Code, Survey question, Possible Answer, store_type, Store Additional Attribute 4</t>
-  </si>
-  <si>
-    <t>Survey</t>
-  </si>
-  <si>
-    <t>POP Agua</t>
-  </si>
-  <si>
-    <t>"Nothing to Tag", "Uniforme", "Corcholata Entrada", "Logo Modelorama Exterior", "Termometro"</t>
-  </si>
-  <si>
-    <t>Nestle, Nestle - Santa Maria, SANTA MARIA</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in at least one of the scene types there is product type POS from brands Nestle, Nestle - Santa Maria, SANTA MARIA, then pass.</t>
-  </si>
-  <si>
-    <t>product_type, exclude skus, manufacturer_name, brand_name, store_type, Store Additional Attribute 4, scene_type</t>
-  </si>
-  <si>
-    <t>Marcas Easy Drinking</t>
-  </si>
-  <si>
-    <t>SKU,Other</t>
-  </si>
-  <si>
-    <t>LIGHT</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Categoria Tradicional "LIGHT" and Manufacturer "ABI-GM", then pass.</t>
-  </si>
-  <si>
-    <t>product_type, manufacturer_name, Categoria Tradicional, store_type, Store Additional Attribute 4, scene_type</t>
-  </si>
-  <si>
-    <t>Exhibicion Adicional</t>
-  </si>
-  <si>
-    <t>Exhibición Adicional: Mega con precio en área de compra</t>
-  </si>
-  <si>
-    <t>Si, No</t>
-  </si>
-  <si>
-    <t>Expected Answers: "Si"</t>
-  </si>
-  <si>
-    <t>Marcas Premium</t>
-  </si>
-  <si>
-    <t>PREMIUM</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Categoria Tradicional "PREMIUM" and Manufacturer "ABI-GM", then pass.</t>
-  </si>
-  <si>
-    <t>Marcas Craft</t>
-  </si>
-  <si>
-    <t>CRAFT &amp; IMPORTS</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Categoria Tradicional "CRAFT &amp; IMPORTS" and Manufacturer "ABI-GM", then pass.</t>
-  </si>
-  <si>
-    <t>Sin Espacios Vacios</t>
-  </si>
-  <si>
-    <t>Empty</t>
-  </si>
-  <si>
-    <t>Share of Empty Spaces: If Empty spaces represent equal or less than 20% of all facings in the visit, then pass.</t>
-  </si>
-  <si>
-    <t>product_type, store_type, Store Additional Attribute 4, scene_type</t>
-  </si>
-  <si>
-    <t>Posters HE/Innovacion/BET</t>
-  </si>
-  <si>
-    <t>SKU, Other</t>
-  </si>
-  <si>
-    <t>2X58 1X33 MEGA CORONA LIGHT, Mega light, Premium Stella Michelob Cucapa_Sabor para conocedores, TendCardTriptico_Michelob, TendCardTriptico_Stella Artois, TendCardTriptico_Cucapa, 1X30MEGAC, 1X28MEGAC, Michelob POS Other, Stella Artois POS Other, Cucapa POS Other</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in at least one of the scene types there is product type POS from selected SKUs, then pass.</t>
-  </si>
-  <si>
-    <t>Product_type, product_name, manufacturer_name, store_type, store Additional Attribue 4, Scene_type</t>
-  </si>
-  <si>
-    <t>Set Botella Abierta</t>
-  </si>
-  <si>
-    <t>BA</t>
-  </si>
-  <si>
-    <t>POP Exterior, POP Interior, Fachada, Exibicion Interna</t>
-  </si>
-  <si>
-    <t>Materiales POCM</t>
-  </si>
-  <si>
-    <t>Materiales POCM (tarros,vasos,dispensador,chalices,cubetas)</t>
-  </si>
-  <si>
-    <t>Question "Materiales POCM (Tarros, Vasos, Dispensadores, Chalices y Cubetas)" If answer is "Si", then pass. </t>
-  </si>
-  <si>
-    <t>Acuerdos Comerciales</t>
-  </si>
-  <si>
-    <t>Cumple acuerdos comerciales (preferencia,promos,webstore)</t>
-  </si>
-  <si>
-    <t>Question "Cumple con acuerdos comerciales, preferencia, promos, web store." If answer is "Si" then pass. </t>
-  </si>
-  <si>
-    <t>Marca Light</t>
-  </si>
-  <si>
-    <t>Exhibición Marca Foco</t>
-  </si>
-  <si>
-    <t>Exhibición Marca foco en barra,contra barra,POP,fachada,mesa</t>
-  </si>
-  <si>
-    <t>Question "Exhibición marca foco en barra, contrabarra, POP, fachada, mesa."  If answer is "Si" then pass.</t>
-  </si>
-  <si>
-    <t>Sin Espacios Vacíos</t>
-  </si>
-  <si>
-    <t>product_type, store_type, Store Additional Attribute 4</t>
-  </si>
-  <si>
-    <t>Set Modeloramas</t>
-  </si>
-  <si>
-    <t>Cigarros</t>
-  </si>
-  <si>
-    <t>Hay o no hay producto?</t>
-  </si>
-  <si>
-    <t>SKU</t>
-  </si>
-  <si>
-    <t>MODELORAMA</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in scene type "Cigarros" there is at least 1 facing for Category "Cigarros", then pass.</t>
-  </si>
-  <si>
-    <t>product type, Category, store_type, scene_type</t>
-  </si>
-  <si>
-    <t>Cooler Vacío</t>
-  </si>
-  <si>
-    <t>SKU,Other, POS</t>
-  </si>
-  <si>
-    <t>100% of Cooler Share must be Product Type SKU or Other. No empty spaces are allowed.</t>
-  </si>
-  <si>
-    <t>product_type, store_type, scene_type</t>
-  </si>
-  <si>
-    <t>Invasión</t>
-  </si>
-  <si>
-    <t>Cerveza, COOLERS, CRAFT &amp; IMPORTS, ENERGIZANTE, LIGHT, PREMIUM, REGULAR, REGULAR/CLARA, REGULAR/OBSCURA, SIN ALCOHOL, VALUE</t>
-  </si>
-  <si>
-    <t>Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the cooler for selected manufacturers and category. 100% purity target.</t>
-  </si>
-  <si>
-    <t>product_type, manufacturer_name, Category, store_type, scene_type</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Manufacturer: "ABI-GM" for Product Type: SKU, then pass.</t>
-  </si>
-  <si>
-    <t>product_type, manufacturer_name, store_type, scene_type</t>
-  </si>
-  <si>
-    <t>Cooler Coca</t>
-  </si>
-  <si>
-    <t>Cooler Coca Cola</t>
-  </si>
-  <si>
-    <t>100% of Cooler Coca Share must be Product Type SKU or Other. No empty spaces are allowed.</t>
-  </si>
-  <si>
-    <t>Coca Cola</t>
-  </si>
-  <si>
-    <t>Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the cooler for selected manufacturer. 100% purity target.</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Manufacturer: "Coca Cola" for Product Type: SKU, then pass.</t>
-  </si>
-  <si>
-    <t>Cooler Pepsi</t>
-  </si>
-  <si>
-    <t>100% of Cooler Pepsi Share must be Product Type SKU or Other. No empty spaces are allowed.</t>
-  </si>
-  <si>
-    <t>Pepsi</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Manufacturer: "Pepsi" for Product Type: SKU, then pass.</t>
-  </si>
-  <si>
-    <t>Galletas</t>
-  </si>
-  <si>
-    <t>Galletas Vacío</t>
-  </si>
-  <si>
-    <t>100% of Galletas Share must be Product Type SKU or Other. No empty spaces are allowed.</t>
-  </si>
-  <si>
-    <t>Gamesa</t>
-  </si>
-  <si>
-    <t>Botana</t>
-  </si>
-  <si>
-    <t>Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the scene type "Galletas" for selected manufacturer "Gamesa" 100% purity target.</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in scene type "Galletas" there is at least 1 facing for Manufacturer "Gamesa" for Product Type: SKU, then pass.</t>
-  </si>
-  <si>
-    <t>Sabritas</t>
-  </si>
-  <si>
-    <t>Sabritas Vacío</t>
-  </si>
-  <si>
-    <t>100% of Share must be Product Type SKU or Other from category "Botana". No empty spaces are allowed.</t>
-  </si>
-  <si>
-    <t>Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the scene type "Sabritas" for selected manufacturer "Sabritas" 100% purity target.</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in scene type "Sabritas" there is at least 1 facing for Manufacturer "Sabritas" for Product Type: SKU, then pass.</t>
-  </si>
-  <si>
-    <t>Logo Modelorama Exterior</t>
-  </si>
-  <si>
-    <t>Hay o no hay logo?</t>
-  </si>
-  <si>
-    <t>At least 1 facing of "Logo Modelorama Exterior" in Scene Type "Logo Modelorama Exterior", then pass.</t>
-  </si>
-  <si>
-    <t>Pop Exterior</t>
-  </si>
-  <si>
-    <t>Hay o no hay Pop?</t>
-  </si>
-  <si>
-    <t>POP Exterior</t>
-  </si>
-  <si>
-    <t>At least 2 facings of :POS" Product type in "POP Exterior" scene type, then pass.</t>
-  </si>
-  <si>
-    <t>Pop Interior</t>
-  </si>
-  <si>
-    <t>POP Interior</t>
-  </si>
-  <si>
-    <t>At least 3 facings of :POS" Product type in "POP Exterior" scene type, then pass.</t>
-  </si>
-  <si>
-    <t>Termometro Exterior</t>
-  </si>
-  <si>
-    <t>Hay o no hay Termometro?</t>
-  </si>
-  <si>
-    <t>Termometro</t>
-  </si>
-  <si>
-    <t>At least 1 facing of "Termometro Exterior" in scene type "Termometro Exterior", then pass.</t>
-  </si>
-  <si>
-    <t>product_type, product_name, store_type, scene_type</t>
-  </si>
-  <si>
-    <t>Uniforme</t>
-  </si>
-  <si>
-    <t>Hay o no hay Uniforme?</t>
-  </si>
-  <si>
-    <t>At least 1 facing of "Uniforme" in scene type "Uniforme", then pass.</t>
-  </si>
-  <si>
-    <t>Set Botella Cerrada Sin Cooler</t>
-  </si>
-  <si>
-    <t>SC</t>
-  </si>
-  <si>
-    <t>Set Botella Abierta Sin Cooler</t>
-  </si>
-  <si>
-    <t>Set Urban</t>
-  </si>
-  <si>
-    <t>URBAN</t>
-  </si>
-  <si>
-    <t>33,66,100</t>
-  </si>
-  <si>
-    <t>CC and SC</t>
-  </si>
-  <si>
-    <t>Fachada, Mesa, Barra</t>
-  </si>
-  <si>
-    <t>Product Availability KPI: If in at least one BRAND POS from Manufacturer ABI is recognized in each scenetype (barra, mesa and fachada), then pass. If one scenetype mentioned is missing or a ABI POS is not recognized into the scenetype the proportional points are lost. The score could be 33%, 66% and 100%</t>
-  </si>
-  <si>
-    <t>product_type, exclude skus, manufacturer_name, store_type, Store Additional Attribute 4, Store Additional Attribute 13, scene_type</t>
-  </si>
-  <si>
-    <t>No te hagas guey</t>
-  </si>
-  <si>
-    <t>NIUNSOLOTRAGO_BOLICHE_COFEPRIS_MODELORAMA
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="187">
+  <si>
+    <t xml:space="preserve">KPI Level 1 Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Level 2 Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Level 3 Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude skus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey Question Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey question</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possible Answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manufacturer_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categoria Tradicional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brand_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store Additional Attribute 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store Additional Attribute 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">template_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pass/Fail Criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">column names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Botella Cerrada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promociones Vigentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POS</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">"Nothing to Tag", "Uniforme", "Corcholata Entrada", "Logo Modelorama Exterior", "Termometro", </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2X58 1X33 MEGA CORONA LIGHT, Mega light, Premium Stella Michelob Cucapa_Sabor para conocedores, TendCardTriptico_Michelob, TendCardTriptico_Stella Artois, TendCardTriptico_Cucapa, 1X30MEGAC, 1X28MEGAC, Michelob POS Other, Stella Artois POS Other, Cucapa POS Other,</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABI-GM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRADICIONAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP Exterior, POP Interior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in at least one of the scene types there is product type POS from Manufacturer ABI, then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, exclude skus, manufacturer_name, store_type, Store Additional Attribute 4, scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pureza Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU,Other,Empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABI-GM, NESTLE, GARCI CRESPO, KERMATO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the cooler for selected manufacturers. 100% purity target.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, manufacturer_name, store_type, Store Additional Attribute 4, scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primer Impacto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enfriador en área alto impacto 100% de productos son de GM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si, No, No tiene Enfriador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Answers: "Si" &amp; "No tiene Enfirador"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey Question Code, Survey question, Possible Answer, store_type, Store Additional Attribute 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Survey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP Agua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Nothing to Tag", "Uniforme", "Corcholata Entrada", "Logo Modelorama Exterior", "Termometro"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nestle, Nestle - Santa Maria, SANTA MARIA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in at least one of the scene types there is product type POS from brands Nestle, Nestle - Santa Maria, SANTA MARIA, then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, exclude skus, manufacturer_name, brand_name, store_type, Store Additional Attribute 4, scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcas Easy Drinking (KPI name changed from Marcas Light)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU,Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIGHT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Categoria Tradicional "LIGHT" and Manufacturer "ABI-GM", then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, manufacturer_name, Categoria Tradicional, store_type, Store Additional Attribute 4, scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exhibicion Adicional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exhibición Adicional: Mega con precio en área de compra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si, No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected Answers: "Si"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcas Premium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREMIUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Categoria Tradicional "PREMIUM" and Manufacturer "ABI-GM", then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcas Craft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRAFT &amp; IMPORTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Categoria Tradicional "CRAFT &amp; IMPORTS" and Manufacturer "ABI-GM", then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin Espacios Vacios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of Empty Spaces: If Empty spaces represent equal or less than 20% of all facings in the visit, then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, store_type, Store Additional Attribute 4, scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Posters HE/Innovacion/BET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU, Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2X58 1X33 MEGA CORONA LIGHT, Mega light, Premium Stella Michelob Cucapa_Sabor para conocedores, TendCardTriptico_Michelob, TendCardTriptico_Stella Artois, TendCardTriptico_Cucapa, 1X30MEGAC, 1X28MEGAC, Michelob POS Other, Stella Artois POS Other, Cucapa POS Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in at least one of the scene types there is product type POS from selected SKUs, then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product_type, product_name, manufacturer_name, store_type, store Additional Attribue 4, Scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Botella Abierta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP Exterior, POP Interior, Fachada, Exibicion Interna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Materiales POCM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Materiales POCM (tarros,vasos,dispensador,chalices,cubetas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question "Materiales POCM (Tarros, Vasos, Dispensadores, Chalices y Cubetas)" If answer is "Si", then pass. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acuerdos Comerciales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cumple acuerdos comerciales (preferencia,promos,webstore)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question "Cumple con acuerdos comerciales, preferencia, promos, web store." If answer is "Si" then pass. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marca Light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exhibición Marca Foco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exhibición Marca foco en barra,contra barra,POP,fachada,mesa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question "Exhibición marca foco en barra, contrabarra, POP, fachada, mesa."  If answer is "Si" then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin Espacios Vacíos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, store_type, Store Additional Attribute 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Modeloramas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cigarros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hay o no hay producto?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MODELORAMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in scene type "Cigarros" there is at least 1 facing for Category "Cigarros", then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product type, Category, store_type, scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler Vacío</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU,Other, POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% of Cooler Share must be Product Type SKU or Other. No empty spaces are allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, store_type, scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invasión</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerveza, COOLERS, CRAFT &amp; IMPORTS, ENERGIZANTE, LIGHT, PREMIUM, REGULAR, REGULAR/CLARA, REGULAR/OBSCURA, SIN ALCOHOL, VALUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the cooler for selected manufacturers and category. 100% purity target.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, manufacturer_name, Category, store_type, scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Manufacturer: "ABI-GM" for Product Type: SKU, then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, manufacturer_name, store_type, scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler Coca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler Coca Cola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% of Cooler Coca Share must be Product Type SKU or Other. No empty spaces are allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca Cola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the cooler for selected manufacturer. 100% purity target.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Manufacturer: "Coca Cola" for Product Type: SKU, then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler Pepsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% of Cooler Pepsi Share must be Product Type SKU or Other. No empty spaces are allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pepsi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in scene type "Cooler" there is at least 1 facing for Manufacturer: "Pepsi" for Product Type: SKU, then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galletas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Galletas Vacío</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% of Galletas Share must be Product Type SKU or Other. No empty spaces are allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gamesa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Botana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the scene type "Galletas" for selected manufacturer "Gamesa" 100% purity target.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in scene type "Galletas" there is at least 1 facing for Manufacturer "Gamesa" for Product Type: SKU, then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sabritas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sabritas Vacío</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100% of Share must be Product Type SKU or Other from category "Botana". No empty spaces are allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purity KPI: Pass if only product type: SKU, OTHER or EMPTY are found in the scene type "Sabritas" for selected manufacturer "Sabritas" 100% purity target.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in scene type "Sabritas" there is at least 1 facing for Manufacturer "Sabritas" for Product Type: SKU, then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logo Modelorama Exterior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hay o no hay logo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least 1 facing of "Logo Modelorama Exterior" in Scene Type "Logo Modelorama Exterior", then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pop Exterior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hay o no hay Pop?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP Exterior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least 2 facings of :POS" Product type in "POP Exterior" scene type, then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pop Interior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POP Interior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least 3 facings of :POS" Product type in "POP Exterior" scene type, then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Termometro Exterior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hay o no hay Termometro?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Termometro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least 1 facing of "Termometro Exterior" in scene type "Termometro Exterior", then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, product_name, store_type, scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uniforme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hay o no hay Uniforme?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least 1 facing of "Uniforme" in scene type "Uniforme", then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Botella Cerrada Sin Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Botella Abierta Sin Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">URBAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC, SC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fachada, Mesa, Barra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability KPI: If in at least one BRAND POS from Manufacturer ABI is recognized in each scenetype (barra, mesa and fachada), then pass. If one scenetype mentioned is missing or a ABI POS is not recognized into the scenetype the proportional points are lost. The score could be 33%, 66% and 100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product_type, exclude skus, manufacturer_name, store_type, Store Additional Attribute 4, Store Additional Attribute 13, scene_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No te hagas guey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIUNSOLOTRAGO_BOLICHE_COFEPRIS_MODELORAMA
 NIUNSOLOTRAGO_JACKPOT_COFEPRIS_MODELORAMA
 NiUnSoloTrago_VARIOS_MODELORAMA
 NOTEHAGASGUEY_+18_MODELORAMA_STICKER_10X18
@@ -550,91 +569,88 @@
 NoTeHagasGuey_VARIOS_Modelorama_POSTER</t>
   </si>
   <si>
-    <t>POP Exterior, POP interior</t>
-  </si>
-  <si>
-    <t>At least 1 facing of the  SKU´s are in scene type "POP Exterior" or "POP Interior", then pass.</t>
-  </si>
-  <si>
-    <t>ticket</t>
-  </si>
-  <si>
-    <t>requerimienrto</t>
-  </si>
-  <si>
-    <t>PS </t>
-  </si>
-  <si>
-    <t>adicionar set nuevo de urban</t>
-  </si>
-  <si>
-    <t>nuevo</t>
-  </si>
-  <si>
-    <t>Todo se hace en la plataforma nueva de xsuite mobile report</t>
-  </si>
-  <si>
-    <t>Pros conf</t>
-  </si>
-  <si>
-    <t>modificar set de modelorama, donde se adiciona el KPI no te hagas wey</t>
-  </si>
-  <si>
-    <t>conf</t>
-  </si>
-  <si>
-    <t>modificar set de BA y BC con reponderacion de puntos, mas atributo adicional </t>
-  </si>
-  <si>
-    <t>Next steps</t>
-  </si>
-  <si>
-    <t>Abrir ticket para migracion de xsuite mobile report </t>
-  </si>
-  <si>
-    <t>Angie</t>
-  </si>
-  <si>
-    <t>Angie pregunta a Felipe de OOB + Custom KPI</t>
-  </si>
-  <si>
-    <t>Crear y adjuntar el template de Rifka (mock up) - URBAN</t>
-  </si>
-  <si>
-    <t>Toño/Charly</t>
-  </si>
-  <si>
-    <t>Crear y adjuntar el template de Rifka (mock up) - No te hagas wey </t>
-  </si>
-  <si>
-    <t>Compartir el nombre de los SKU no te hagas wey </t>
-  </si>
-  <si>
-    <t>Vico</t>
-  </si>
-  <si>
-    <t>Compartir el listado de los clientes que tienen cooler en atributo 13 (0/1)</t>
-  </si>
-  <si>
-    <t>Abrir tickets pros de configuracion de nuevos KPIs</t>
-  </si>
-  <si>
-    <t>fix nombres de column names porque estan mal (exlude vs. exclude)</t>
-  </si>
-  <si>
-    <t>remove "weights" from column names</t>
-  </si>
-  <si>
-    <t>arreglar las que dicen categoria y poner Categoria Tradicional</t>
-  </si>
-  <si>
-    <t>it nos not called scene_type it is template_name</t>
-  </si>
-  <si>
-    <t>store type 1</t>
-  </si>
-  <si>
-    <t>store type 2</t>
+    <t xml:space="preserve">POP Exterior, POP interior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least 1 facing of the  SKU´s are in scene type "POP Exterior" or "POP Interior", then pass.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ticket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">requerimienrto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">adicionar set nuevo de urban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuevo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todo se hace en la plataforma nueva de xsuite mobile report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pros conf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modificar set de modelorama, donde se adiciona el KPI no te hagas wey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modificar set de BA y BC con reponderacion de puntos, mas atributo adicional </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next steps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abrir ticket para migracion de xsuite mobile report </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angie pregunta a Felipe de OOB + Custom KPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear y adjuntar el template de Rifka (mock up) - URBAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toño/Charly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crear y adjuntar el template de Rifka (mock up) - No te hagas wey </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compartir el nombre de los SKU no te hagas wey </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compartir el listado de los clientes que tienen cooler en atributo 13 (0/1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abrir tickets pros de configuracion de nuevos KPIs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fix nombres de column names porque estan mal (exlude vs. exclude)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remove "weights" from column names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arreglar las que dicen categoria y poner Categoria Tradicional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it nos not called scene_type it is template_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store type</t>
   </si>
 </sst>
 </file>
@@ -642,9 +658,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -689,6 +705,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -704,7 +728,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -727,6 +751,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
   </fills>
@@ -778,7 +808,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -800,6 +830,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -831,12 +865,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -863,7 +905,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -921,7 +963,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFC000"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -950,37 +992,37 @@
   </sheetPr>
   <dimension ref="A1:U65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P13" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q49" activeCellId="0" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="40.3622448979592"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="117.714285714286"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="71.5459183673469"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="39.9591836734694"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="116.362244897959"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="70.734693877551"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="22" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1045,17 +1087,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="C2" s="0" t="str">
+        <f aca="false">B2</f>
+        <v>Promociones Vigentes</v>
+      </c>
       <c r="D2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -1082,7 +1128,7 @@
       <c r="M2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="6" t="n">
+      <c r="N2" s="7" t="n">
         <v>40</v>
       </c>
       <c r="O2" s="0" t="s">
@@ -1091,13 +1137,13 @@
       <c r="P2" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="9" t="s">
         <v>31</v>
       </c>
       <c r="T2" s="0" t="s">
@@ -1107,13 +1153,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="C3" s="0" t="str">
+        <f aca="false">B3</f>
+        <v>Pureza Cooler</v>
+      </c>
       <c r="D3" s="0" t="s">
         <v>35</v>
       </c>
@@ -1138,13 +1188,13 @@
       <c r="P3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="9" t="s">
         <v>38</v>
       </c>
       <c r="T3" s="0" t="s">
@@ -1161,6 +1211,10 @@
       <c r="B4" s="0" t="s">
         <v>41</v>
       </c>
+      <c r="C4" s="0" t="str">
+        <f aca="false">B4</f>
+        <v>Primer Impacto</v>
+      </c>
       <c r="D4" s="0" t="s">
         <v>25</v>
       </c>
@@ -1191,13 +1245,13 @@
       <c r="P4" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="Q4" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R4" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="S4" s="9" t="s">
         <v>44</v>
       </c>
       <c r="T4" s="0" t="s">
@@ -1214,6 +1268,10 @@
       <c r="B5" s="0" t="s">
         <v>47</v>
       </c>
+      <c r="C5" s="0" t="str">
+        <f aca="false">B5</f>
+        <v>POP Agua</v>
+      </c>
       <c r="D5" s="0" t="s">
         <v>23</v>
       </c>
@@ -1241,13 +1299,13 @@
       <c r="P5" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="S5" s="10" t="s">
         <v>50</v>
       </c>
       <c r="T5" s="0" t="s">
@@ -1261,8 +1319,12 @@
       <c r="A6" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="6" t="s">
         <v>52</v>
+      </c>
+      <c r="C6" s="0" t="str">
+        <f aca="false">B6</f>
+        <v>Marcas Easy Drinking (KPI name changed from Marcas Light)</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>53</v>
@@ -1288,29 +1350,33 @@
       <c r="P6" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="Q6" s="7" t="s">
+      <c r="Q6" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="S6" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="T6" s="10" t="s">
+      <c r="T6" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="U6" s="10" t="s">
+      <c r="U6" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="C7" s="0" t="str">
+        <f aca="false">B7</f>
+        <v>Exhibicion Adicional</v>
+      </c>
       <c r="D7" s="0" t="s">
         <v>25</v>
       </c>
@@ -1341,19 +1407,19 @@
       <c r="P7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="Q7" s="7" t="s">
+      <c r="Q7" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R7" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="S7" s="8" t="s">
+      <c r="S7" s="9" t="s">
         <v>60</v>
       </c>
       <c r="T7" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="U7" s="10" t="s">
+      <c r="U7" s="11" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1364,6 +1430,10 @@
       <c r="B8" s="0" t="s">
         <v>61</v>
       </c>
+      <c r="C8" s="0" t="str">
+        <f aca="false">B8</f>
+        <v>Marcas Premium</v>
+      </c>
       <c r="D8" s="0" t="s">
         <v>53</v>
       </c>
@@ -1388,19 +1458,19 @@
       <c r="P8" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="Q8" s="7" t="s">
+      <c r="Q8" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R8" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S8" s="9" t="s">
+      <c r="S8" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="T8" s="10" t="s">
+      <c r="T8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="U8" s="10" t="s">
+      <c r="U8" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1411,6 +1481,10 @@
       <c r="B9" s="0" t="s">
         <v>64</v>
       </c>
+      <c r="C9" s="0" t="str">
+        <f aca="false">B9</f>
+        <v>Marcas Craft</v>
+      </c>
       <c r="D9" s="0" t="s">
         <v>53</v>
       </c>
@@ -1435,19 +1509,19 @@
       <c r="P9" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="Q9" s="7" t="s">
+      <c r="Q9" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R9" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S9" s="9" t="s">
+      <c r="S9" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="T9" s="10" t="s">
+      <c r="T9" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="U9" s="10" t="s">
+      <c r="U9" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1458,6 +1532,10 @@
       <c r="B10" s="0" t="s">
         <v>67</v>
       </c>
+      <c r="C10" s="0" t="str">
+        <f aca="false">B10</f>
+        <v>Sin Espacios Vacios</v>
+      </c>
       <c r="D10" s="0" t="s">
         <v>68</v>
       </c>
@@ -1482,16 +1560,16 @@
       <c r="P10" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="Q10" s="7" t="s">
+      <c r="Q10" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R10" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S10" s="9" t="s">
+      <c r="S10" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="T10" s="11" t="s">
+      <c r="T10" s="12" t="s">
         <v>70</v>
       </c>
       <c r="U10" s="0" t="s">
@@ -1499,62 +1577,74 @@
       </c>
     </row>
     <row r="11" s="5" customFormat="true" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="C11" s="6" t="str">
+        <f aca="false">B11</f>
+        <v>Posters HE/Innovacion/BET</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="E11" s="6"/>
+      <c r="F11" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="10" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="N11" s="5" t="n">
+      <c r="K11" s="6"/>
+      <c r="L11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="6" t="n">
         <v>10</v>
       </c>
-      <c r="O11" s="10" t="s">
+      <c r="O11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P11" s="10" t="s">
+      <c r="P11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="Q11" s="7" t="s">
+      <c r="Q11" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R11" s="10" t="s">
+      <c r="R11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="S11" s="9" t="s">
+      <c r="S11" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="T11" s="11" t="s">
+      <c r="T11" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="U11" s="10" t="s">
+      <c r="U11" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>76</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="C12" s="0" t="str">
+        <f aca="false">B12</f>
+        <v>Promociones Vigentes</v>
+      </c>
       <c r="D12" s="0" t="s">
         <v>23</v>
       </c>
@@ -1582,13 +1672,13 @@
       <c r="P12" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="Q12" s="7" t="s">
+      <c r="Q12" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R12" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="S12" s="8" t="s">
+      <c r="S12" s="9" t="s">
         <v>31</v>
       </c>
       <c r="T12" s="0" t="s">
@@ -1598,13 +1688,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>76</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="C13" s="0" t="str">
+        <f aca="false">B13</f>
+        <v>Pureza Cooler</v>
+      </c>
       <c r="D13" s="0" t="s">
         <v>35</v>
       </c>
@@ -1629,13 +1723,13 @@
       <c r="P13" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="Q13" s="7" t="s">
+      <c r="Q13" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R13" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S13" s="8" t="s">
+      <c r="S13" s="9" t="s">
         <v>38</v>
       </c>
       <c r="T13" s="0" t="s">
@@ -1645,13 +1739,17 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>76</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>79</v>
       </c>
+      <c r="C14" s="0" t="str">
+        <f aca="false">B14</f>
+        <v>Materiales POCM</v>
+      </c>
       <c r="D14" s="0" t="s">
         <v>25</v>
       </c>
@@ -1682,13 +1780,13 @@
       <c r="P14" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="Q14" s="7" t="s">
+      <c r="Q14" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R14" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="S14" s="8" t="s">
+      <c r="S14" s="9" t="s">
         <v>81</v>
       </c>
       <c r="T14" s="0" t="s">
@@ -1698,13 +1796,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>76</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>82</v>
       </c>
+      <c r="C15" s="0" t="str">
+        <f aca="false">B15</f>
+        <v>Acuerdos Comerciales</v>
+      </c>
       <c r="D15" s="0" t="s">
         <v>25</v>
       </c>
@@ -1735,13 +1837,13 @@
       <c r="P15" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="Q15" s="7" t="s">
+      <c r="Q15" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R15" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="S15" s="8" t="s">
+      <c r="S15" s="9" t="s">
         <v>84</v>
       </c>
       <c r="T15" s="0" t="s">
@@ -1758,6 +1860,10 @@
       <c r="B16" s="0" t="s">
         <v>85</v>
       </c>
+      <c r="C16" s="0" t="str">
+        <f aca="false">B16</f>
+        <v>Marca Light</v>
+      </c>
       <c r="D16" s="0" t="s">
         <v>53</v>
       </c>
@@ -1773,7 +1879,7 @@
       <c r="M16" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="N16" s="5" t="n">
+      <c r="N16" s="6" t="n">
         <v>5</v>
       </c>
       <c r="O16" s="0" t="s">
@@ -1782,29 +1888,33 @@
       <c r="P16" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="Q16" s="7" t="s">
+      <c r="Q16" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R16" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S16" s="9" t="s">
+      <c r="S16" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="T16" s="10" t="s">
+      <c r="T16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="U16" s="10" t="s">
+      <c r="U16" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>76</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>86</v>
       </c>
+      <c r="C17" s="0" t="str">
+        <f aca="false">B17</f>
+        <v>Exhibición Marca Foco</v>
+      </c>
       <c r="D17" s="0" t="s">
         <v>25</v>
       </c>
@@ -1835,13 +1945,13 @@
       <c r="P17" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="Q17" s="7" t="s">
+      <c r="Q17" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R17" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="S17" s="8" t="s">
+      <c r="S17" s="9" t="s">
         <v>88</v>
       </c>
       <c r="T17" s="0" t="s">
@@ -1858,6 +1968,10 @@
       <c r="B18" s="0" t="s">
         <v>89</v>
       </c>
+      <c r="C18" s="0" t="str">
+        <f aca="false">B18</f>
+        <v>Sin Espacios Vacíos</v>
+      </c>
       <c r="D18" s="0" t="s">
         <v>68</v>
       </c>
@@ -1882,23 +1996,23 @@
       <c r="P18" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="Q18" s="7" t="s">
+      <c r="Q18" s="8" t="s">
         <v>29</v>
       </c>
       <c r="R18" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S18" s="9" t="s">
+      <c r="S18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="T18" s="11" t="s">
+      <c r="T18" s="12" t="s">
         <v>90</v>
       </c>
       <c r="U18" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>91</v>
       </c>
@@ -1935,13 +2049,13 @@
       <c r="O19" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P19" s="0" t="s">
+      <c r="P19" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R19" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="S19" s="9" t="s">
+      <c r="S19" s="10" t="s">
         <v>96</v>
       </c>
       <c r="T19" s="0" t="s">
@@ -1951,7 +2065,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>91</v>
       </c>
@@ -1988,23 +2102,23 @@
       <c r="O20" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P20" s="0" t="s">
+      <c r="P20" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R20" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S20" s="9" t="s">
+      <c r="S20" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="T20" s="11" t="s">
+      <c r="T20" s="12" t="s">
         <v>101</v>
       </c>
       <c r="U20" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>91</v>
       </c>
@@ -2041,23 +2155,23 @@
       <c r="O21" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P21" s="0" t="s">
+      <c r="P21" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R21" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S21" s="9" t="s">
+      <c r="S21" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="T21" s="13" t="s">
+      <c r="T21" s="17" t="s">
         <v>105</v>
       </c>
       <c r="U21" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>91</v>
       </c>
@@ -2094,13 +2208,13 @@
       <c r="O22" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P22" s="0" t="s">
+      <c r="P22" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R22" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S22" s="9" t="s">
+      <c r="S22" s="10" t="s">
         <v>106</v>
       </c>
       <c r="T22" s="0" t="s">
@@ -2110,7 +2224,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>91</v>
       </c>
@@ -2147,23 +2261,23 @@
       <c r="O23" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P23" s="0" t="s">
+      <c r="P23" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R23" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="S23" s="9" t="s">
+      <c r="S23" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="T23" s="11" t="s">
+      <c r="T23" s="12" t="s">
         <v>101</v>
       </c>
       <c r="U23" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>91</v>
       </c>
@@ -2200,23 +2314,23 @@
       <c r="O24" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P24" s="0" t="s">
+      <c r="P24" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R24" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="S24" s="9" t="s">
+      <c r="S24" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="T24" s="13" t="s">
+      <c r="T24" s="17" t="s">
         <v>107</v>
       </c>
       <c r="U24" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>91</v>
       </c>
@@ -2253,13 +2367,13 @@
       <c r="O25" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P25" s="0" t="s">
+      <c r="P25" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R25" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="S25" s="9" t="s">
+      <c r="S25" s="10" t="s">
         <v>113</v>
       </c>
       <c r="T25" s="0" t="s">
@@ -2269,7 +2383,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>91</v>
       </c>
@@ -2306,23 +2420,23 @@
       <c r="O26" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P26" s="0" t="s">
+      <c r="P26" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R26" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="S26" s="9" t="s">
+      <c r="S26" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="T26" s="11" t="s">
+      <c r="T26" s="12" t="s">
         <v>101</v>
       </c>
       <c r="U26" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>91</v>
       </c>
@@ -2359,23 +2473,23 @@
       <c r="O27" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P27" s="0" t="s">
+      <c r="P27" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R27" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="S27" s="9" t="s">
+      <c r="S27" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="T27" s="13" t="s">
+      <c r="T27" s="17" t="s">
         <v>107</v>
       </c>
       <c r="U27" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>91</v>
       </c>
@@ -2412,13 +2526,13 @@
       <c r="O28" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P28" s="0" t="s">
+      <c r="P28" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R28" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="S28" s="9" t="s">
+      <c r="S28" s="10" t="s">
         <v>117</v>
       </c>
       <c r="T28" s="0" t="s">
@@ -2428,7 +2542,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>91</v>
       </c>
@@ -2459,23 +2573,23 @@
       <c r="O29" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P29" s="0" t="s">
+      <c r="P29" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R29" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="S29" s="9" t="s">
+      <c r="S29" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="T29" s="11" t="s">
+      <c r="T29" s="12" t="s">
         <v>101</v>
       </c>
       <c r="U29" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>91</v>
       </c>
@@ -2512,23 +2626,23 @@
       <c r="O30" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P30" s="0" t="s">
+      <c r="P30" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R30" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="S30" s="9" t="s">
+      <c r="S30" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="T30" s="13" t="s">
+      <c r="T30" s="17" t="s">
         <v>105</v>
       </c>
       <c r="U30" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>91</v>
       </c>
@@ -2565,23 +2679,23 @@
       <c r="O31" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P31" s="0" t="s">
+      <c r="P31" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R31" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="S31" s="9" t="s">
+      <c r="S31" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="T31" s="13" t="s">
+      <c r="T31" s="17" t="s">
         <v>105</v>
       </c>
       <c r="U31" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>91</v>
       </c>
@@ -2612,23 +2726,23 @@
       <c r="O32" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P32" s="0" t="s">
+      <c r="P32" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R32" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="S32" s="9" t="s">
+      <c r="S32" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="T32" s="11" t="s">
+      <c r="T32" s="12" t="s">
         <v>101</v>
       </c>
       <c r="U32" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>91</v>
       </c>
@@ -2659,23 +2773,23 @@
       <c r="O33" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P33" s="0" t="s">
+      <c r="P33" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R33" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="S33" s="9" t="s">
+      <c r="S33" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="T33" s="13" t="s">
+      <c r="T33" s="17" t="s">
         <v>105</v>
       </c>
       <c r="U33" s="0" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>91</v>
       </c>
@@ -2706,16 +2820,16 @@
       <c r="O34" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P34" s="0" t="s">
+      <c r="P34" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R34" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="S34" s="9" t="s">
+      <c r="S34" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="T34" s="13" t="s">
+      <c r="T34" s="17" t="s">
         <v>105</v>
       </c>
       <c r="U34" s="0" t="s">
@@ -2759,7 +2873,7 @@
       <c r="O35" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P35" s="0" t="s">
+      <c r="P35" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R35" s="0" t="s">
@@ -2768,7 +2882,7 @@
       <c r="S35" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="T35" s="11" t="s">
+      <c r="T35" s="12" t="s">
         <v>101</v>
       </c>
       <c r="U35" s="0" t="s">
@@ -2812,7 +2926,7 @@
       <c r="O36" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P36" s="0" t="s">
+      <c r="P36" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R36" s="0" t="s">
@@ -2821,7 +2935,7 @@
       <c r="S36" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="T36" s="11" t="s">
+      <c r="T36" s="12" t="s">
         <v>101</v>
       </c>
       <c r="U36" s="0" t="s">
@@ -2865,7 +2979,7 @@
       <c r="O37" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P37" s="0" t="s">
+      <c r="P37" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R37" s="0" t="s">
@@ -2874,7 +2988,7 @@
       <c r="S37" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="T37" s="11" t="s">
+      <c r="T37" s="12" t="s">
         <v>101</v>
       </c>
       <c r="U37" s="0" t="s">
@@ -2915,13 +3029,13 @@
       <c r="M38" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="N38" s="7" t="n">
+      <c r="N38" s="8" t="n">
         <v>5</v>
       </c>
       <c r="O38" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P38" s="0" t="s">
+      <c r="P38" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R38" s="0" t="s">
@@ -2930,7 +3044,7 @@
       <c r="S38" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="T38" s="11" t="s">
+      <c r="T38" s="12" t="s">
         <v>144</v>
       </c>
       <c r="U38" s="0" t="s">
@@ -2977,7 +3091,7 @@
       <c r="O39" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="P39" s="0" t="s">
+      <c r="P39" s="16" t="s">
         <v>95</v>
       </c>
       <c r="R39" s="0" t="s">
@@ -2986,586 +3100,621 @@
       <c r="S39" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="T39" s="11" t="s">
+      <c r="T39" s="12" t="s">
         <v>144</v>
       </c>
       <c r="U39" s="0" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N40" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B42" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7" t="s">
+      <c r="C42" s="0" t="str">
+        <f aca="false">B42</f>
+        <v>Promociones Vigentes</v>
+      </c>
+      <c r="D42" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E42" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F40" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J40" s="7" t="s">
+      <c r="F42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J42" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K40" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L40" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M40" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N40" s="7" t="n">
+      <c r="K42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N42" s="8" t="n">
         <v>62</v>
       </c>
-      <c r="O40" s="7" t="s">
+      <c r="O42" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P40" s="7" t="s">
+      <c r="P42" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q40" s="7" t="s">
+      <c r="Q42" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="R40" s="7" t="s">
+      <c r="R42" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="S40" s="15" t="s">
+      <c r="S42" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="T40" s="7" t="s">
+      <c r="T42" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="U40" s="7" t="s">
+      <c r="U42" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="s">
+    <row r="43" customFormat="false" ht="24.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B43" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7" t="s">
+      <c r="C43" s="0" t="str">
+        <f aca="false">B43</f>
+        <v>POP Agua</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E43" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7" t="s">
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M41" s="7" t="s">
+      <c r="K43" s="8"/>
+      <c r="L43" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M43" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="N41" s="7" t="n">
+      <c r="N43" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="O41" s="7" t="s">
+      <c r="O43" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P41" s="7" t="s">
+      <c r="P43" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q41" s="7" t="s">
+      <c r="Q43" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="R41" s="7" t="s">
+      <c r="R43" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="S41" s="16" t="s">
+      <c r="S43" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="T41" s="7" t="s">
+      <c r="T43" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="U41" s="7" t="s">
+      <c r="U43" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="s">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B44" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7" t="n">
+      <c r="C44" s="0" t="str">
+        <f aca="false">B44</f>
+        <v>Exhibicion Adicional</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="H42" s="7" t="s">
+      <c r="H44" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="I42" s="7" t="s">
+      <c r="I44" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="J42" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M42" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N42" s="7" t="n">
+      <c r="J44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N44" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="O42" s="7" t="s">
+      <c r="O44" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P42" s="7" t="s">
+      <c r="P44" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q42" s="7" t="s">
+      <c r="Q44" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="R42" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="S42" s="15" t="s">
+      <c r="R44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S44" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="T42" s="7" t="s">
+      <c r="T44" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="U42" s="7" t="s">
+      <c r="U44" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
+    <row r="45" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B45" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="7"/>
-      <c r="D43" s="7" t="s">
+      <c r="C45" s="0" t="str">
+        <f aca="false">B45</f>
+        <v>Posters HE/Innovacion/BET</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E43" s="7"/>
-      <c r="F43" s="17" t="s">
+      <c r="E45" s="8"/>
+      <c r="F45" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7" t="s">
+      <c r="G45" s="8"/>
+      <c r="H45" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M43" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N43" s="7" t="n">
+      <c r="K45" s="8"/>
+      <c r="L45" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M45" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N45" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="O43" s="7" t="s">
+      <c r="O45" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P43" s="7" t="s">
+      <c r="P45" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="Q43" s="7" t="s">
+      <c r="Q45" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="R43" s="7" t="s">
+      <c r="R45" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="S43" s="16" t="s">
+      <c r="S45" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="T43" s="18" t="s">
+      <c r="T45" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="U43" s="7" t="s">
+      <c r="U45" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="s">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B46" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7" t="s">
+      <c r="C46" s="0" t="str">
+        <f aca="false">B46</f>
+        <v>Promociones Vigentes</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E46" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7" t="s">
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M44" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N44" s="7" t="n">
+      <c r="K46" s="8"/>
+      <c r="L46" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M46" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N46" s="8" t="n">
         <v>58</v>
       </c>
-      <c r="O44" s="7" t="s">
+      <c r="O46" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P44" s="7" t="s">
+      <c r="P46" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="Q44" s="7" t="s">
+      <c r="Q46" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="R44" s="7" t="s">
+      <c r="R46" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="S44" s="15" t="s">
+      <c r="S46" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="T44" s="7" t="s">
+      <c r="T46" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="U44" s="7" t="s">
+      <c r="U46" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B47" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7" t="n">
+      <c r="C47" s="0" t="str">
+        <f aca="false">B47</f>
+        <v>Materiales POCM</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="H45" s="7" t="s">
+      <c r="H47" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="I45" s="7" t="s">
+      <c r="I47" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="J45" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M45" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N45" s="7" t="n">
+      <c r="J47" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K47" s="8"/>
+      <c r="L47" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M47" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N47" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="O45" s="7" t="s">
+      <c r="O47" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P45" s="7" t="s">
+      <c r="P47" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="Q45" s="7" t="s">
+      <c r="Q47" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="R45" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="S45" s="15" t="s">
+      <c r="R47" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S47" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="T45" s="7" t="s">
+      <c r="T47" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="U45" s="7" t="s">
+      <c r="U47" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="s">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B48" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="7"/>
-      <c r="D46" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7" t="n">
+      <c r="C48" s="0" t="str">
+        <f aca="false">B48</f>
+        <v>Acuerdos Comerciales</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="H46" s="7" t="s">
+      <c r="H48" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="I46" s="7" t="s">
+      <c r="I48" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="J46" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M46" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N46" s="7" t="n">
+      <c r="J48" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K48" s="8"/>
+      <c r="L48" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M48" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N48" s="8" t="n">
         <v>18</v>
       </c>
-      <c r="O46" s="7" t="s">
+      <c r="O48" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P46" s="7" t="s">
+      <c r="P48" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="Q46" s="7" t="s">
+      <c r="Q48" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="R46" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="S46" s="15" t="s">
+      <c r="R48" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S48" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="T46" s="7" t="s">
+      <c r="T48" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="U46" s="7" t="s">
+      <c r="U48" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
+    <row r="49" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B49" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7" t="n">
+      <c r="C49" s="0" t="str">
+        <f aca="false">B49</f>
+        <v>Exhibición Marca Foco</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="H47" s="7" t="s">
+      <c r="H49" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="I47" s="7" t="s">
+      <c r="I49" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="J47" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K47" s="7"/>
-      <c r="L47" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M47" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N47" s="7" t="n">
+      <c r="J49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K49" s="8"/>
+      <c r="L49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N49" s="8" t="n">
         <v>18</v>
       </c>
-      <c r="O47" s="7" t="s">
+      <c r="O49" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P47" s="7" t="s">
+      <c r="P49" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="Q47" s="7" t="s">
+      <c r="Q49" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="R47" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="S47" s="15" t="s">
+      <c r="R49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S49" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="T47" s="7" t="s">
+      <c r="T49" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="U47" s="7" t="s">
+      <c r="U49" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="s">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B50" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7" t="s">
+      <c r="C50" s="0" t="str">
+        <f aca="false">B50</f>
+        <v>URBAN</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E50" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I48" s="7"/>
-      <c r="J48" s="7" t="s">
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K48" s="7"/>
-      <c r="L48" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M48" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N48" s="7" t="s">
+      <c r="K50" s="8"/>
+      <c r="L50" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N50" s="8" t="n">
+        <v>100</v>
+      </c>
+      <c r="O50" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P50" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q50" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="O48" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="P48" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q48" s="7" t="s">
+      <c r="R50" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="R48" s="7" t="s">
+      <c r="S50" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="S48" s="15" t="s">
+      <c r="T50" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="T48" s="7" t="s">
+      <c r="U50" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="26.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="U48" s="7" t="s">
+      <c r="C51" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="8"/>
+      <c r="F51" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N51" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="O51" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="P51" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="R51" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="S51" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="T51" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="U51" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="23.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E49" s="7"/>
-      <c r="F49" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I49" s="7"/>
-      <c r="J49" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K49" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L49" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M49" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N49" s="7" t="n">
-        <v>5</v>
-      </c>
-      <c r="O49" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="P49" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q49" s="7"/>
-      <c r="R49" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="S49" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="T49" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="U49" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:U49"/>
+  <autoFilter ref="A1:U50"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3591,111 +3740,111 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="63.1785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="C2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="23" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="20" t="s">
+      <c r="C3" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="D3" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="E3" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="23" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="20" t="s">
+      <c r="C4" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="D4" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="D4" s="0" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>171</v>
-      </c>
       <c r="D5" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="E9" s="0" t="s">
         <v>174</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>179</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3722,7 +3871,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3748,28 +3897,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="50.0816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3788,30 +3937,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="B1" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" s="0" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>